<commit_message>
Journal de bord totalement complété
</commit_message>
<xml_diff>
--- a/Journal de bord.xlsx
+++ b/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\site_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6135AEF6-C0B2-4F36-844C-6B94C7A0F284}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9F9E11-C508-4AE5-AAB6-F8B491547E84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="125">
   <si>
     <t>Elisa</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Mise en archive</t>
   </si>
   <si>
-    <t>Déplacement des pages lisp, pascal, PHP, types_langage,</t>
-  </si>
-  <si>
     <t>Changements des liens footer et menu</t>
   </si>
   <si>
@@ -370,6 +367,39 @@
   </si>
   <si>
     <t>Corrections, ajout sources, paragraphe Java, ajout de liens dans le menu et dans le footer</t>
+  </si>
+  <si>
+    <t>Déplacement des pages lisp, pascal, PHP, types_langage</t>
+  </si>
+  <si>
+    <t>Ajout d'une image JPG shéma monde IA</t>
+  </si>
+  <si>
+    <t>Changement de la couleur de la classe code</t>
+  </si>
+  <si>
+    <t>Remise en forme du code</t>
+  </si>
+  <si>
+    <t>Renomination de l'image JPG shéma monde IA</t>
+  </si>
+  <si>
+    <t>Non respect des conventions (espaces)</t>
+  </si>
+  <si>
+    <t>Modification du script JS</t>
+  </si>
+  <si>
+    <t>Remise en forme du code et ajout d'instructions pour la fonction info</t>
+  </si>
+  <si>
+    <t>Transformation des styles page a en a</t>
+  </si>
+  <si>
+    <t>Création de la fonction explication</t>
+  </si>
+  <si>
+    <t>Insertion d'appel à la fct explication pr certains mots</t>
   </si>
 </sst>
 </file>
@@ -699,11 +729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,7 +1812,7 @@
         <v>44182</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>84</v>
@@ -1805,7 +1835,7 @@
         <v>81</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>2</v>
@@ -1822,10 +1852,10 @@
         <v>44189</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>2</v>
@@ -1842,7 +1872,7 @@
         <v>44189</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>84</v>
@@ -1862,10 +1892,10 @@
         <v>44189</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>2</v>
@@ -1882,7 +1912,7 @@
         <v>44191</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>17</v>
@@ -1891,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>16</v>
@@ -1902,10 +1932,10 @@
         <v>44195</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>2</v>
@@ -1922,10 +1952,10 @@
         <v>44195</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>2</v>
@@ -1942,7 +1972,7 @@
         <v>44195</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>53</v>
@@ -1962,7 +1992,7 @@
         <v>44195</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>84</v>
@@ -1982,7 +2012,7 @@
         <v>44195</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>17</v>
@@ -1991,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>16</v>
@@ -2002,10 +2032,10 @@
         <v>44195</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>2</v>
@@ -2022,7 +2052,7 @@
         <v>44195</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>53</v>
@@ -2042,10 +2072,10 @@
         <v>44195</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>2</v>
@@ -2062,10 +2092,10 @@
         <v>44195</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>2</v>
@@ -2082,10 +2112,10 @@
         <v>44196</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>2</v>
@@ -2102,7 +2132,7 @@
         <v>44196</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>53</v>
@@ -2122,10 +2152,10 @@
         <v>44197</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>2</v>
@@ -2142,10 +2172,10 @@
         <v>44197</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>2</v>
@@ -2162,10 +2192,10 @@
         <v>44197</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>2</v>
@@ -2182,10 +2212,10 @@
         <v>44197</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>2</v>
@@ -2202,10 +2232,10 @@
         <v>44197</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>2</v>
@@ -2222,10 +2252,10 @@
         <v>44197</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>2</v>
@@ -2242,10 +2272,10 @@
         <v>44197</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>2</v>
@@ -2262,18 +2292,178 @@
         <v>44197</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="2" t="s">
+      <c r="C81" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>44202</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>43841</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>43841</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>43841</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Journal de bord
</commit_message>
<xml_diff>
--- a/Journal de bord.xlsx
+++ b/Journal de bord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\site_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B878013-6851-4336-93AA-CF4A345115E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253E37C6-F423-4466-A9B9-71DBE88D4B70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="133">
   <si>
     <t>Elisa</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>Modification de la page robotique</t>
+  </si>
+  <si>
+    <t>Modification des pages contact, intelligence_artificielle et robotique</t>
   </si>
 </sst>
 </file>
@@ -765,11 +768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,17 +2626,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>44209</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D94" s="5">
-        <f>COUNTIF(D1:D92,"Mathieu")/91*100</f>
-        <v>91.208791208791212</v>
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="5">
+        <f>COUNTIF(D1:D93,"Mathieu")/92*100</f>
+        <v>91.304347826086953</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F86" xr:uid="{7DF5F1E6-1B6D-45B9-909D-ACA50CA9F9F9}"/>
+  <autoFilter ref="A1:F93" xr:uid="{7DF5F1E6-1B6D-45B9-909D-ACA50CA9F9F9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>